<commit_message>
Added types to the structure file
</commit_message>
<xml_diff>
--- a/DB Table Layout CSVs/Structure.xlsx
+++ b/DB Table Layout CSVs/Structure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwbh1\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwbh1\Git\ClementsComponents\DB Table Layout CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F2097836-30B8-460F-B1A8-6603EBC56889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C4A3742-BB7E-4D59-A9DE-9C0C799550C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25725" yWindow="945" windowWidth="28305" windowHeight="18915" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="19" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="107">
   <si>
     <t>id</t>
   </si>
@@ -361,6 +361,21 @@
   </si>
   <si>
     <t>Write Time</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>bool</t>
   </si>
 </sst>
 </file>
@@ -423,6 +438,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -722,15 +741,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C56DEE4B-35B7-4840-A352-F90FFD092ED1}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V4" sqref="A2:V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -829,6 +848,90 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>106</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -836,15 +939,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D49EDD-7BE0-40E6-A3A8-150559F158C9}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -952,6 +1055,96 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -959,15 +1152,15 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38390A0-54F1-4DE8-8480-A8B57FD51327}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1079,6 +1272,99 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1088,13 +1374,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C800FFF8-EB63-4D13-A531-2DA66EB7DC38}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1194,6 +1480,90 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>106</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="N9" s="1"/>
     </row>
@@ -1204,15 +1574,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9937C9-D72E-7D4C-8D11-F954FDD4B477}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1304,6 +1674,84 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>106</v>
+      </c>
+      <c r="V2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1311,15 +1759,15 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74009144-6000-4DCE-ADC8-643CDEB204CB}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1423,6 +1871,93 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1430,15 +1965,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977C67C8-6511-471B-8F67-51435D018A4E}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1542,6 +2077,93 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1549,15 +2171,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81D82F8-684D-4252-BDD2-B1BD99628C59}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1661,6 +2283,93 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1668,15 +2377,15 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D0861D-FF3B-4E9D-8156-3B95E4271E68}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M8:M9"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1779,6 +2488,93 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1786,15 +2582,15 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9D9773-5D29-4823-9865-AC8804846EE5}">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1898,6 +2694,93 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1905,15 +2788,15 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED86387E-96F5-427A-97CB-34A75A2EB5CA}">
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:X4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2013,6 +2896,90 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>106</v>
+      </c>
+      <c r="X2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2020,15 +2987,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD3EA12-FBE1-534B-A058-44EBBDB29AD3}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2104,6 +3071,72 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2111,15 +3144,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33662F3B-BCFF-4120-9B3D-AE2E385CBC31}">
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:Z4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2227,6 +3260,96 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>105</v>
+      </c>
+      <c r="W2" t="s">
+        <v>105</v>
+      </c>
+      <c r="X2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>106</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2234,15 +3357,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D7AFB1-4B0E-B341-B58C-DB56D25AB17F}">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2322,6 +3445,75 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>106</v>
+      </c>
+      <c r="S2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2329,15 +3521,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F5E1FC-E905-E645-BF1D-9F825CBAA9FA}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2421,6 +3613,78 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>106</v>
+      </c>
+      <c r="T2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2430,13 +3694,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40477AF-F08B-4B2D-AAF3-3AF01CF0F23D}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2524,6 +3788,81 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>106</v>
+      </c>
+      <c r="U2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>39</v>
@@ -2536,15 +3875,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29238628-6433-4A2D-8D83-5848109D5E04}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2636,6 +3975,84 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>106</v>
+      </c>
+      <c r="V2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2643,15 +4060,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A53F0F9-78DA-5E4F-8CE4-A8328C6349C1}">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2743,6 +4160,84 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>106</v>
+      </c>
+      <c r="V2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2750,15 +4245,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE76E14-ED57-9743-A015-2A8C14FF7037}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2854,6 +4349,87 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>106</v>
+      </c>
+      <c r="W2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2861,15 +4437,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0DE0CA-698D-344A-B15B-8FB5812A7204}">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -2965,6 +4541,87 @@
         <v>23</v>
       </c>
     </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>106</v>
+      </c>
+      <c r="W2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated to include Op-Amps
Also added a kindly GPT4o generated script for creating tables from the CSVs
</commit_message>
<xml_diff>
--- a/DB Table Layout CSVs/Structure.xlsx
+++ b/DB Table Layout CSVs/Structure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwbh1\Git\ClementsComponents\DB Table Layout CSVs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Clement Hathaway\GitHub\ClementsComponents\DB Table Layout CSVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C4A3742-BB7E-4D59-A9DE-9C0C799550C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C61668-4F1E-4A95-A2F4-837E6E953552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25725" yWindow="945" windowWidth="28305" windowHeight="18915" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="33480" windowHeight="20985" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="19" r:id="rId1"/>
@@ -18,21 +18,22 @@
     <sheet name="Capacitors" sheetId="2" r:id="rId3"/>
     <sheet name="Inductors" sheetId="3" r:id="rId4"/>
     <sheet name="Diodes" sheetId="17" r:id="rId5"/>
-    <sheet name="LEDs" sheetId="18" r:id="rId6"/>
-    <sheet name="BJTs" sheetId="4" r:id="rId7"/>
-    <sheet name="MOSFETs" sheetId="5" r:id="rId8"/>
-    <sheet name="IGBTs" sheetId="6" r:id="rId9"/>
-    <sheet name="Analog ICs" sheetId="10" r:id="rId10"/>
-    <sheet name="Sensor ICs" sheetId="13" r:id="rId11"/>
-    <sheet name="Sensors" sheetId="20" r:id="rId12"/>
-    <sheet name="Digital ICs" sheetId="7" r:id="rId13"/>
-    <sheet name="PMICs" sheetId="11" r:id="rId14"/>
-    <sheet name="Power Drivers" sheetId="14" r:id="rId15"/>
-    <sheet name="Protection ICs" sheetId="15" r:id="rId16"/>
-    <sheet name="Communication ICs" sheetId="12" r:id="rId17"/>
-    <sheet name="MCUs" sheetId="8" r:id="rId18"/>
-    <sheet name="Clocks and Crystals" sheetId="16" r:id="rId19"/>
-    <sheet name="Memory" sheetId="9" r:id="rId20"/>
+    <sheet name="Op-Amps" sheetId="21" r:id="rId6"/>
+    <sheet name="LEDs" sheetId="18" r:id="rId7"/>
+    <sheet name="BJTs" sheetId="4" r:id="rId8"/>
+    <sheet name="MOSFETs" sheetId="5" r:id="rId9"/>
+    <sheet name="IGBTs" sheetId="6" r:id="rId10"/>
+    <sheet name="Analog ICs" sheetId="10" r:id="rId11"/>
+    <sheet name="Sensor ICs" sheetId="13" r:id="rId12"/>
+    <sheet name="Sensors" sheetId="20" r:id="rId13"/>
+    <sheet name="Digital ICs" sheetId="7" r:id="rId14"/>
+    <sheet name="PMICs" sheetId="11" r:id="rId15"/>
+    <sheet name="Power Drivers" sheetId="14" r:id="rId16"/>
+    <sheet name="Protection ICs" sheetId="15" r:id="rId17"/>
+    <sheet name="Communication ICs" sheetId="12" r:id="rId18"/>
+    <sheet name="MCUs" sheetId="8" r:id="rId19"/>
+    <sheet name="Clocks and Crystals" sheetId="16" r:id="rId20"/>
+    <sheet name="Memory" sheetId="9" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="110">
   <si>
     <t>id</t>
   </si>
@@ -376,6 +377,15 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>Slew Rate</t>
+  </si>
+  <si>
+    <t>Input Offset Voltage</t>
+  </si>
+  <si>
+    <t>Input Bias Current</t>
   </si>
 </sst>
 </file>
@@ -440,14 +450,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -485,7 +491,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -591,7 +597,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -733,7 +739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -938,6 +944,198 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0DE0CA-698D-344A-B15B-8FB5812A7204}">
+  <dimension ref="A1:W4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>105</v>
+      </c>
+      <c r="R2" t="s">
+        <v>105</v>
+      </c>
+      <c r="S2" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
+        <v>105</v>
+      </c>
+      <c r="V2" t="s">
+        <v>106</v>
+      </c>
+      <c r="W2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D49EDD-7BE0-40E6-A3A8-150559F158C9}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
@@ -1150,7 +1348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38390A0-54F1-4DE8-8480-A8B57FD51327}">
   <dimension ref="A1:AA4"/>
   <sheetViews>
@@ -1370,7 +1568,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C800FFF8-EB63-4D13-A531-2DA66EB7DC38}">
   <dimension ref="A1:X9"/>
   <sheetViews>
@@ -1572,7 +1770,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9937C9-D72E-7D4C-8D11-F954FDD4B477}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -1757,7 +1955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74009144-6000-4DCE-ADC8-643CDEB204CB}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -1963,7 +2161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{977C67C8-6511-471B-8F67-51435D018A4E}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -2169,7 +2367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81D82F8-684D-4252-BDD2-B1BD99628C59}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -2375,7 +2573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D0861D-FF3B-4E9D-8156-3B95E4271E68}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -2580,7 +2778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F9D9773-5D29-4823-9865-AC8804846EE5}">
   <dimension ref="A1:Y4"/>
   <sheetViews>
@@ -2786,7 +2984,164 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD3EA12-FBE1-534B-A058-44EBBDB29AD3}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>106</v>
+      </c>
+      <c r="R2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED86387E-96F5-427A-97CB-34A75A2EB5CA}">
   <dimension ref="A1:X4"/>
   <sheetViews>
@@ -2985,164 +3340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DD3EA12-FBE1-534B-A058-44EBBDB29AD3}">
-  <dimension ref="A1:R4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>106</v>
-      </c>
-      <c r="R2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33662F3B-BCFF-4120-9B3D-AE2E385CBC31}">
   <dimension ref="A1:Z4"/>
   <sheetViews>
@@ -3359,8 +3557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D7AFB1-4B0E-B341-B58C-DB56D25AB17F}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3694,7 +3892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40477AF-F08B-4B2D-AAF3-3AF01CF0F23D}">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
@@ -3874,6 +4072,103 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B18DB20-8240-40CD-9FA5-43BC839B46CC}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L1" t="s">
+        <v>6</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29238628-6433-4A2D-8D83-5848109D5E04}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -4058,7 +4353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A53F0F9-78DA-5E4F-8CE4-A8328C6349C1}">
   <dimension ref="A1:V4"/>
   <sheetViews>
@@ -4243,7 +4538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE76E14-ED57-9743-A015-2A8C14FF7037}">
   <dimension ref="A1:W4"/>
   <sheetViews>
@@ -4433,196 +4728,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE0DE0CA-698D-344A-B15B-8FB5812A7204}">
-  <dimension ref="A1:W4"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F2" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" t="s">
-        <v>105</v>
-      </c>
-      <c r="K2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M2" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>105</v>
-      </c>
-      <c r="R2" t="s">
-        <v>105</v>
-      </c>
-      <c r="S2" t="s">
-        <v>105</v>
-      </c>
-      <c r="T2" t="s">
-        <v>105</v>
-      </c>
-      <c r="U2" t="s">
-        <v>105</v>
-      </c>
-      <c r="V2" t="s">
-        <v>106</v>
-      </c>
-      <c r="W2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>